<commit_message>
lin_reg added to airbnb, airbnb eda refactored to eda, test 19 now brings best radj to 41.97. Next step is PCA
</commit_message>
<xml_diff>
--- a/regressions.xlsx
+++ b/regressions.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Initial Test (18)</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>13+a30</t>
+  </si>
+  <si>
+    <t>13+a30-accommodates (br only)</t>
   </si>
 </sst>
 </file>
@@ -463,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.58203125" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -542,128 +545,128 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1">
-        <v>0.44253382708567301</v>
+        <v>0.26769751295559902</v>
       </c>
       <c r="D4" s="1">
-        <v>0.31941486167725602</v>
+        <v>-4.3707193623551898E+17</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1">
-        <v>0.43380942994413102</v>
+        <v>0.33828500531767502</v>
       </c>
       <c r="D5" s="1">
-        <v>0.30629208457081503</v>
+        <v>-2.3764335247271301E+19</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1">
-        <v>0.279378997880327</v>
+        <v>0.28398595974829299</v>
       </c>
       <c r="D6" s="1">
-        <v>0.26613508941716602</v>
+        <v>-2.4469840680783299E+18</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1">
-        <v>0.282021334533677</v>
+        <v>0.21087938195358999</v>
       </c>
       <c r="D7" s="1">
-        <v>0.23276875538546099</v>
+        <v>0.21152648495421</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
       <c r="C8" s="1">
-        <v>0.21087938195358999</v>
+        <v>0.279378997880327</v>
       </c>
       <c r="D8" s="1">
-        <v>0.21152648495421</v>
+        <v>0.26613508941716602</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="1">
-        <v>1.5964593767525698E-2</v>
+        <v>0.282021334533677</v>
       </c>
       <c r="D9" s="1">
-        <v>-5.5768233534769698E-3</v>
+        <v>0.23276875538546099</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C10" s="1">
-        <v>0.26769751295559902</v>
+        <v>1.5964593767525698E-2</v>
       </c>
       <c r="D10" s="1">
-        <v>-4.3707193623551898E+17</v>
+        <v>-5.5768233534769698E-3</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1">
-        <v>0.28398595974829299</v>
+        <v>0.44253382708567301</v>
       </c>
       <c r="D11" s="1">
-        <v>-2.4469840680783299E+18</v>
+        <v>0.31941486167725602</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C12" s="1">
-        <v>0.33828500531767502</v>
+        <v>0.43380942994413102</v>
       </c>
       <c r="D12" s="1">
-        <v>-2.3764335247271301E+19</v>
+        <v>0.30629208457081503</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -743,10 +746,21 @@
         <v>0.41101850695791697</v>
       </c>
     </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.41968152389993701</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D1">
-    <sortState ref="A2:D12">
-      <sortCondition descending="1" ref="D1"/>
+    <sortState ref="A2:D19">
+      <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
1. Dropped High prices that were throwing off the Random Forest model (30 outliers) Price limited to 700 and below. 2. Ran city vs zipcode. City determined nothing so dropped. 3. Created Travis price per person variables. 4. Created babr dummy variable that is bedrooms plus bathrooms 5. Created a for loop to make visualizations of price vs every other column as scatter and histogram. 6. Created a report results with error where results is radjustedsquare 7. Drop max minimum nights to 31 because one results had a 180 night minimum. 8. updated gitignore.
</commit_message>
<xml_diff>
--- a/regressions.xlsx
+++ b/regressions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="36" windowWidth="22224" windowHeight="9528"/>
+    <workbookView xWindow="384" yWindow="96" windowWidth="22224" windowHeight="9468"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Initial Test (18)</t>
   </si>
@@ -95,16 +95,54 @@
   </si>
   <si>
     <t>13+a30-accommodates (br only)</t>
+  </si>
+  <si>
+    <t>Test 19 with prices over 699 dropped</t>
+  </si>
+  <si>
+    <t>RF</t>
+  </si>
+  <si>
+    <t>KNN</t>
+  </si>
+  <si>
+    <t>Test 20 is t19 - city - comfort</t>
+  </si>
+  <si>
+    <t>Test 24 babr var</t>
+  </si>
+  <si>
+    <t>Test 21 price 1 p/acc</t>
+  </si>
+  <si>
+    <t>Test 22 price 2 p/beds</t>
+  </si>
+  <si>
+    <t>Test 23 price 3 p/brs</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Intercept</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="14"/>
       <color theme="1"/>
@@ -130,15 +168,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -466,24 +507,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.58203125" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.9140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.9140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.58203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.08203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.4140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.58203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.08203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.58203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -497,16 +545,28 @@
         <v>14</v>
       </c>
       <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -519,17 +579,29 @@
       <c r="D2" s="1">
         <v>0.32639912950567901</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="3">
+        <v>134.65</v>
+      </c>
+      <c r="F2" s="3">
+        <v>-145.71</v>
+      </c>
+      <c r="G2">
         <v>0.32600000000000001</v>
       </c>
-      <c r="F2" s="2">
+      <c r="H2">
         <v>0.32600000000000001</v>
       </c>
-      <c r="G2" s="2">
+      <c r="I2">
         <v>0.30099999999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J2" s="1">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="K2" s="2">
+        <v>3.6999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -542,8 +614,11 @@
       <c r="D3" s="1">
         <v>0.32036063861196701</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -556,8 +631,11 @@
       <c r="D4" s="1">
         <v>-4.3707193623551898E+17</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -570,8 +648,11 @@
       <c r="D5" s="1">
         <v>-2.3764335247271301E+19</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -584,8 +665,11 @@
       <c r="D6" s="1">
         <v>-2.4469840680783299E+18</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -598,8 +682,11 @@
       <c r="D7" s="1">
         <v>0.21152648495421</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -612,8 +699,11 @@
       <c r="D8" s="1">
         <v>0.26613508941716602</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -626,8 +716,11 @@
       <c r="D9" s="1">
         <v>0.23276875538546099</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -640,8 +733,11 @@
       <c r="D10" s="1">
         <v>-5.5768233534769698E-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -654,8 +750,11 @@
       <c r="D11" s="1">
         <v>0.31941486167725602</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -668,8 +767,11 @@
       <c r="D12" s="1">
         <v>0.30629208457081503</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -679,8 +781,11 @@
       <c r="D13" s="1">
         <v>1.5518227999758299E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -690,8 +795,11 @@
       <c r="D14" s="1">
         <v>0.40451360902823302</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -701,8 +809,11 @@
       <c r="D15" s="1">
         <v>0.29739705994795401</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -712,8 +823,11 @@
       <c r="D16" s="1">
         <v>0.28642174078905702</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -723,8 +837,11 @@
       <c r="D17" s="1">
         <v>0.28337076783382698</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -734,8 +851,11 @@
       <c r="D18" s="1">
         <v>0.282523811730017</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -745,8 +865,11 @@
       <c r="D19" s="1">
         <v>0.41101850695791697</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -755,6 +878,129 @@
       </c>
       <c r="D20" s="1">
         <v>0.41968152389993701</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.46159999999999995</v>
+      </c>
+      <c r="E21" s="3">
+        <v>72.099999999999994</v>
+      </c>
+      <c r="F21" s="3">
+        <v>-37.71</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0.52059999999999995</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.47570000000000001</v>
+      </c>
+      <c r="E22" s="3">
+        <v>72.12</v>
+      </c>
+      <c r="F22" s="3">
+        <v>-19.399999999999999</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0.53349999999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.195293361006104</v>
+      </c>
+      <c r="E23" s="3">
+        <v>21.95</v>
+      </c>
+      <c r="F23" s="3">
+        <v>44.228264488395197</v>
+      </c>
+      <c r="J23" s="1">
+        <v>0.21640000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.40760000000000002</v>
+      </c>
+      <c r="E24" s="3">
+        <v>48.03</v>
+      </c>
+      <c r="F24" s="3">
+        <v>89.09</v>
+      </c>
+      <c r="J24" s="1">
+        <v>0.5101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.4758</v>
+      </c>
+      <c r="E25" s="3">
+        <v>72.12</v>
+      </c>
+      <c r="F25" s="3">
+        <v>-19.399999999999999</v>
+      </c>
+      <c r="J25" s="1">
+        <v>0.53359999999999996</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0.47799999999999998</v>
+      </c>
+      <c r="E26" s="3">
+        <v>72.040000000000006</v>
+      </c>
+      <c r="F26" s="3">
+        <v>-10.48</v>
+      </c>
+      <c r="J26" s="1">
+        <v>0.51659999999999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>